<commit_message>
added system project and glossary to Resources
</commit_message>
<xml_diff>
--- a/resources/Resources.xlsx
+++ b/resources/Resources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janro\Desktop\KN-Spectrum_E-moto\.github\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janro\Desktop\Summertime Project\.github\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33737D74-3586-4796-A3F9-07FC6841A861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE739CFF-F49D-4D7E-B7CA-AB99633C4F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>Kraków</t>
   </si>
@@ -181,6 +181,21 @@
   </si>
   <si>
     <t>GPS6MV2</t>
+  </si>
+  <si>
+    <t>Glossary</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>Integrated Circuit</t>
+  </si>
+  <si>
+    <t>MicroControler Unit</t>
+  </si>
+  <si>
+    <t>Single board computer</t>
   </si>
 </sst>
 </file>
@@ -204,10 +219,28 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -216,8 +249,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -236,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{274D851F-288D-41B3-91DF-C8AEB89CD367}" name="Tabela2" displayName="Tabela2" ref="A1:H38" totalsRowShown="0">
-  <autoFilter ref="A1:H38" xr:uid="{274D851F-288D-41B3-91DF-C8AEB89CD367}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{274D851F-288D-41B3-91DF-C8AEB89CD367}" name="Tabela2" displayName="Tabela2" ref="A1:H450" totalsRowShown="0">
+  <autoFilter ref="A1:H450" xr:uid="{274D851F-288D-41B3-91DF-C8AEB89CD367}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{2DB4BCF3-0F54-4A6F-BEFA-4E9AD0DB69F2}" name="Place"/>
     <tableColumn id="14" xr3:uid="{678CB6B4-86AC-4397-9676-80221BEB6F0B}" name="Owner"/>
@@ -515,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,9 +570,11 @@
     <col min="6" max="7" width="23.5703125" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -556,8 +599,12 @@
       <c r="H1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -582,8 +629,10 @@
       <c r="H2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -608,8 +657,14 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -634,8 +689,14 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -660,8 +721,14 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -686,8 +753,10 @@
       <c r="H6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -709,8 +778,10 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -732,8 +803,10 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -755,8 +828,10 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="2"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -775,8 +850,10 @@
       <c r="G10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -792,8 +869,10 @@
       <c r="E11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="2"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -815,8 +894,10 @@
       <c r="H12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="2"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -838,8 +919,10 @@
       <c r="G13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="2"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -861,8 +944,10 @@
       <c r="G14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="2"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -884,8 +969,10 @@
       <c r="G15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="2"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -904,8 +991,33 @@
       <c r="G16">
         <v>1</v>
       </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="2"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="2"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="2"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+      <c r="K21" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>